<commit_message>
Changed from pos/neg to 1/0
</commit_message>
<xml_diff>
--- a/data/output/vader/vader_tesla.xlsx
+++ b/data/output/vader/vader_tesla.xlsx
@@ -13102,10 +13102,10 @@
     <t>let, optimistic, tesla, production, model, every, car, let, generous, k, thats, pessimisticvalue, million, profit, million, good, week, burning, cash</t>
   </si>
   <si>
-    <t>pos</t>
-  </si>
-  <si>
-    <t>neg</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>

</xml_diff>